<commit_message>
Changes not staged for commit: 	modified:   actual_items.xlsx 	modified:   stock_analysis.ipynb 	modified:   stock_analysis.xlsx 	modified:   time_series_10_22.pkl
</commit_message>
<xml_diff>
--- a/actual_items.xlsx
+++ b/actual_items.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="116">
   <si>
     <t>Контрактная площадка</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>production_line</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>2 stage</t>
   </si>
 </sst>
 </file>
@@ -728,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B108"/>
+  <dimension ref="A1:B109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,16 +755,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
+      <c r="A2" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -766,7 +772,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
@@ -774,7 +780,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
@@ -782,7 +788,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -790,7 +796,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>2</v>
@@ -798,7 +804,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -806,7 +812,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>2</v>
@@ -814,23 +820,23 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>2</v>
@@ -838,7 +844,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
@@ -846,7 +852,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>2</v>
@@ -854,7 +860,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>2</v>
@@ -862,7 +868,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
@@ -870,7 +876,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>2</v>
@@ -878,7 +884,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>2</v>
@@ -886,7 +892,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>2</v>
@@ -894,7 +900,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>2</v>
@@ -902,7 +908,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>2</v>
@@ -910,7 +916,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>2</v>
@@ -918,7 +924,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>2</v>
@@ -926,7 +932,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>2</v>
@@ -934,7 +940,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>2</v>
@@ -942,7 +948,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
@@ -950,7 +956,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>2</v>
@@ -958,7 +964,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>2</v>
@@ -966,7 +972,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>2</v>
@@ -974,7 +980,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>2</v>
@@ -982,7 +988,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>2</v>
@@ -990,7 +996,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>2</v>
@@ -998,7 +1004,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>2</v>
@@ -1006,7 +1012,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>2</v>
@@ -1014,7 +1020,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>2</v>
@@ -1022,7 +1028,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>2</v>
@@ -1030,7 +1036,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>2</v>
@@ -1038,7 +1044,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>2</v>
@@ -1046,7 +1052,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>2</v>
@@ -1054,7 +1060,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>2</v>
@@ -1062,15 +1068,15 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>49</v>
@@ -1078,15 +1084,15 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>57</v>
@@ -1094,7 +1100,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>57</v>
@@ -1102,7 +1108,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>57</v>
@@ -1110,7 +1116,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>57</v>
@@ -1118,7 +1124,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>57</v>
@@ -1126,7 +1132,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>57</v>
@@ -1134,7 +1140,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>57</v>
@@ -1142,23 +1148,23 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>57</v>
@@ -1166,7 +1172,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>57</v>
@@ -1174,15 +1180,15 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>102</v>
@@ -1190,15 +1196,15 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>49</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>49</v>
@@ -1206,7 +1212,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>49</v>
@@ -1214,7 +1220,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>49</v>
@@ -1222,15 +1228,15 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>57</v>
@@ -1238,7 +1244,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>57</v>
@@ -1246,7 +1252,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>57</v>
@@ -1254,15 +1260,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>102</v>
@@ -1270,7 +1276,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>102</v>
@@ -1278,15 +1284,15 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>57</v>
@@ -1294,7 +1300,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>94</v>
+        <v>66</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>57</v>
@@ -1302,23 +1308,23 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>57</v>
@@ -1326,7 +1332,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>57</v>
@@ -1334,7 +1340,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>67</v>
+        <v>96</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>57</v>
@@ -1342,23 +1348,23 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>57</v>
@@ -1366,7 +1372,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>57</v>
@@ -1374,7 +1380,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>57</v>
@@ -1382,7 +1388,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>57</v>
@@ -1390,7 +1396,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>57</v>
@@ -1398,7 +1404,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>57</v>
@@ -1406,7 +1412,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>57</v>
@@ -1414,7 +1420,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>57</v>
@@ -1422,7 +1428,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>57</v>
@@ -1430,7 +1436,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>57</v>
@@ -1438,7 +1444,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>57</v>
@@ -1446,7 +1452,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>57</v>
@@ -1454,7 +1460,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>57</v>
@@ -1462,7 +1468,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>57</v>
@@ -1470,39 +1476,39 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>57</v>
@@ -1510,7 +1516,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>57</v>
@@ -1518,7 +1524,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>57</v>
@@ -1526,7 +1532,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>57</v>
@@ -1534,7 +1540,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>57</v>
@@ -1542,15 +1548,15 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>2</v>
+        <v>57</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>2</v>
@@ -1558,7 +1564,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>2</v>
@@ -1566,7 +1572,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>2</v>
@@ -1574,7 +1580,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>2</v>
@@ -1582,7 +1588,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>2</v>
@@ -1590,7 +1596,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>2</v>
@@ -1598,9 +1604,17 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B108" s="1" t="s">
+      <c r="B109" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>